<commit_message>
rapport f and PPT
</commit_message>
<xml_diff>
--- a/Rapport/Gant/diagram_gant_Planifié.xlsx
+++ b/Rapport/Gant/diagram_gant_Planifié.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Etude supérieur\S8\PFA\AdminDashboard\Rapport\Gant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PFA_PROJET\BackOfficeDashboard\Rapport\Gant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360FF5A0-8BFC-414B-A4ED-D6A55E24B638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183ECED2-2C98-4BC7-95F7-CB242B354540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="660" yWindow="2325" windowWidth="11640" windowHeight="7875" xr2:uid="{EC0BE597-1989-4C44-8F91-2FD10F983B3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EC0BE597-1989-4C44-8F91-2FD10F983B3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,9 +30,6 @@
     <t>Tâches</t>
   </si>
   <si>
-    <t>Date Debut</t>
-  </si>
-  <si>
     <t>Date Fin</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">Implementation de la sécurité </t>
+  </si>
+  <si>
+    <t>Date Début</t>
   </si>
 </sst>
 </file>
@@ -136,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +154,22 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,19 +201,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,7 +279,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -557,400 +575,683 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C310ED2-D0E1-4C5E-946A-79B528BD19D3}">
-  <dimension ref="A2:Q20"/>
+  <dimension ref="A2:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="49.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="17" width="8.7109375" customWidth="1"/>
+    <col min="6" max="17" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <f>DATE(2024, 2, 29)</f>
         <v>45351</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5">
+        <f ca="1">TODAY()</f>
+        <v>45440</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45439</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <f ca="1">INT((B4 -B3)/7)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="6">
+      <c r="F7" s="2">
         <f>B3</f>
         <v>45351</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="2">
         <f>F7+ 7</f>
         <v>45358</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="2">
         <f t="shared" ref="H7:Q7" si="0">G7+ 7</f>
         <v>45365</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
         <v>45372</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="2">
         <f t="shared" si="0"/>
         <v>45379</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="2">
         <f t="shared" si="0"/>
         <v>45386</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="2">
         <f t="shared" si="0"/>
         <v>45393</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="2">
         <f t="shared" si="0"/>
         <v>45400</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="2">
         <f t="shared" si="0"/>
         <v>45407</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="2">
         <f t="shared" si="0"/>
         <v>45414</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="2">
         <f t="shared" si="0"/>
         <v>45421</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="2">
         <f t="shared" si="0"/>
         <v>45428</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f>B3</f>
         <v>45351</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <f>$B9 +7</f>
         <v>45358</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <f>(C9 -B9)</f>
         <v>7</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="7">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="6">
         <f>B9+7</f>
         <v>45358</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <f t="shared" ref="C10:C20" si="1">$B10 +7</f>
         <v>45365</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>7</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="7">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6">
         <f t="shared" ref="B11:B20" si="2">B10+7</f>
         <v>45365</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <f t="shared" si="1"/>
         <v>45372</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>7</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="6">
         <f t="shared" si="2"/>
         <v>45372</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <f t="shared" si="1"/>
         <v>45379</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <f>(C12 -B12)</f>
         <v>7</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="7">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="6">
         <f t="shared" si="2"/>
         <v>45379</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <f t="shared" si="1"/>
         <v>45386</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <f t="shared" ref="D13:D20" si="3">(C13 -B13)</f>
         <v>7</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="7">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6">
         <f t="shared" si="2"/>
         <v>45386</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <f t="shared" si="1"/>
         <v>45393</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="7">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6">
         <f t="shared" si="2"/>
         <v>45393</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <f t="shared" si="1"/>
         <v>45400</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="7">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6">
         <f t="shared" si="2"/>
         <v>45400</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <f t="shared" si="1"/>
         <v>45407</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="7">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="6">
         <f t="shared" si="2"/>
         <v>45407</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <f t="shared" si="1"/>
         <v>45414</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="7">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="6">
         <f t="shared" si="2"/>
         <v>45414</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <f t="shared" si="1"/>
         <v>45421</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="7">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+    </row>
+    <row r="19" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="6">
         <f t="shared" si="2"/>
         <v>45421</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <f t="shared" si="1"/>
         <v>45428</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="7">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="6">
         <f t="shared" si="2"/>
         <v>45428</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <f t="shared" si="1"/>
         <v>45435</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="7">
         <v>0</v>
       </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>